<commit_message>
slf in blocks table to 1:6
</commit_message>
<xml_diff>
--- a/blocks.xlsx
+++ b/blocks.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D9AE7F-03E6-4D6F-8F3E-DA0B4FABCE84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5DD59A-84DD-4F28-8F4C-3D90FB05BB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
 Lõpetuseks küsime sinult veel mõned küsimused.</t>
   </si>
   <si>
-    <t>1:4</t>
-  </si>
-  <si>
     <t>Kognitiivse efektiivsuse mõõtmise plokk:</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>0:0</t>
+  </si>
+  <si>
+    <t>1:6</t>
   </si>
 </sst>
 </file>
@@ -446,8 +446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,13 +482,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="225" customHeight="1" x14ac:dyDescent="0.25">
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -589,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -647,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -763,7 +763,7 @@
         <v>-1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -792,7 +792,7 @@
         <v>-1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -821,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -908,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -937,7 +937,7 @@
         <v>-1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -966,7 +966,7 @@
         <v>-1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1024,7 +1024,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I21">
         <v>0</v>

</xml_diff>

<commit_message>
slf in blocks table to 1:7
</commit_message>
<xml_diff>
--- a/blocks.xlsx
+++ b/blocks.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5DD59A-84DD-4F28-8F4C-3D90FB05BB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63AC16F-3CD9-4DE7-8703-2D4A24D53B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t>0:0</t>
   </si>
   <si>
-    <t>1:6</t>
+    <t>1:7</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
lisasin lause, et fb kestus on fikseeritud
</commit_message>
<xml_diff>
--- a/blocks.xlsx
+++ b/blocks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A814D1-769E-4B22-A399-5417B2DB7C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A897CC8B-8E4C-4DBF-850C-140F2CF8F3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
   <si>
     <t>Katses kuvatakse aeg-ajalt tagasisidet, mis võtab arvesse nii täpsust kui kiirust.
 Täpsemalt näed, mitmest protsendist inimestest sinu sooritus tõenäoliselt parem oli. Tagasiside aluseks olevad võrdlusandmed pärinevad sama katse sooritajatel USA-s.
-Järgmise ülesande lõpus näed ka tagasisidet.</t>
+Järgmise ülesande lõpus näed ka tagasisidet. Katses on tagasiside kestus fikseeritud, kuid prooviseeriatel aitab nendest edasi liikuda katse läbiviija.</t>
   </si>
 </sst>
 </file>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>

</xml_diff>